<commit_message>
update example values and units
</commit_message>
<xml_diff>
--- a/templates/dataplant/CIMR/CIMR_-_Chromatography.xlsx
+++ b/templates/dataplant/CIMR/CIMR_-_Chromatography.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="173">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -374,6 +374,9 @@
     <t>Parameter [flow rate]</t>
   </si>
   <si>
+    <t xml:space="preserve">Unit    </t>
+  </si>
+  <si>
     <t>Term Source REF (PATO:0001574)</t>
   </si>
   <si>
@@ -515,7 +518,13 @@
     <t>Acetonitrile + 0.1% formic acid</t>
   </si>
   <si>
-    <t>300 nL/min</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Milliliter per Minute</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/NCIT:C64777</t>
   </si>
   <si>
     <t>1 bar</t>
@@ -577,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:CB2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:CB2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:CC2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:CC2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -659,8 +668,9 @@
     <filterColumn colId="77" hiddenButton="1"/>
     <filterColumn colId="78" hiddenButton="1"/>
     <filterColumn colId="79" hiddenButton="1"/>
+    <filterColumn colId="80" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="80">
+  <tableColumns count="81">
     <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Parameter [sample resuspension]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (DPBO:0000169)" totalsRowFunction="none"/>
@@ -730,17 +740,18 @@
     <tableColumn id="67" name="Term Source REF (DPBO:0000139)" totalsRowFunction="none"/>
     <tableColumn id="68" name="Term Accession Number (DPBO:0000139)" totalsRowFunction="none"/>
     <tableColumn id="69" name="Parameter [flow rate]" totalsRowFunction="none"/>
-    <tableColumn id="70" name="Term Source REF (PATO:0001574)" totalsRowFunction="none"/>
-    <tableColumn id="71" name="Term Accession Number (PATO:0001574)" totalsRowFunction="none"/>
-    <tableColumn id="72" name="Parameter [chromatography pressure]" totalsRowFunction="none"/>
-    <tableColumn id="73" name="Term Source REF (DPBO:0000166)" totalsRowFunction="none"/>
-    <tableColumn id="74" name="Term Accession Number (DPBO:0000166)" totalsRowFunction="none"/>
-    <tableColumn id="75" name="Parameter [chromatography gradient]" totalsRowFunction="none"/>
-    <tableColumn id="76" name="Term Source REF (DPBO:0000081)" totalsRowFunction="none"/>
-    <tableColumn id="77" name="Term Accession Number (DPBO:0000081)" totalsRowFunction="none"/>
-    <tableColumn id="78" name="Output [Data]" totalsRowFunction="none"/>
-    <tableColumn id="79" name="Data Format" totalsRowFunction="none"/>
-    <tableColumn id="80" name="Data Selector Format" totalsRowFunction="none"/>
+    <tableColumn id="70" name="Unit    " totalsRowFunction="none"/>
+    <tableColumn id="71" name="Term Source REF (PATO:0001574)" totalsRowFunction="none"/>
+    <tableColumn id="72" name="Term Accession Number (PATO:0001574)" totalsRowFunction="none"/>
+    <tableColumn id="73" name="Parameter [chromatography pressure]" totalsRowFunction="none"/>
+    <tableColumn id="74" name="Term Source REF (DPBO:0000166)" totalsRowFunction="none"/>
+    <tableColumn id="75" name="Term Accession Number (DPBO:0000166)" totalsRowFunction="none"/>
+    <tableColumn id="76" name="Parameter [chromatography gradient]" totalsRowFunction="none"/>
+    <tableColumn id="77" name="Term Source REF (DPBO:0000081)" totalsRowFunction="none"/>
+    <tableColumn id="78" name="Term Accession Number (DPBO:0000081)" totalsRowFunction="none"/>
+    <tableColumn id="79" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="80" name="Data Format" totalsRowFunction="none"/>
+    <tableColumn id="81" name="Data Selector Format" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1274,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CB2"/>
+  <dimension ref="A1:CC2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1518,247 +1529,253 @@
       <c r="CB1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="CC1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" t="s">
+        <v>132</v>
+      </c>
+      <c r="P2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" t="s">
+        <v>132</v>
+      </c>
+      <c r="T2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U2" t="s">
+        <v>132</v>
+      </c>
+      <c r="V2" t="s">
+        <v>132</v>
+      </c>
+      <c r="W2" t="s">
+        <v>142</v>
+      </c>
+      <c r="X2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD2" t="s">
         <v>133</v>
       </c>
-      <c r="D2" t="s">
+      <c r="AE2" t="s">
         <v>134</v>
       </c>
-      <c r="E2" t="s">
+      <c r="AF2" t="s">
         <v>135</v>
       </c>
-      <c r="F2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M2" t="s">
-        <v>131</v>
-      </c>
-      <c r="N2" t="s">
-        <v>138</v>
-      </c>
-      <c r="O2" t="s">
-        <v>131</v>
-      </c>
-      <c r="P2" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>139</v>
-      </c>
-      <c r="R2" t="s">
-        <v>131</v>
-      </c>
-      <c r="S2" t="s">
-        <v>131</v>
-      </c>
-      <c r="T2" t="s">
-        <v>140</v>
-      </c>
-      <c r="U2" t="s">
-        <v>131</v>
-      </c>
-      <c r="V2" t="s">
-        <v>131</v>
-      </c>
-      <c r="W2" t="s">
-        <v>141</v>
-      </c>
-      <c r="X2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AG2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU2" t="s">
         <v>144</v>
       </c>
-      <c r="AA2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>143</v>
-      </c>
       <c r="AV2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AW2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AX2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AY2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AZ2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="BA2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="BB2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="BC2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="BD2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="BE2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="BF2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="BG2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BH2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BI2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="BK2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="BL2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BM2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BN2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BO2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BP2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BQ2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="BR2" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="BS2" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="BT2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="BU2" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="BV2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BW2" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="BX2" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="BY2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BZ2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="CA2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="CB2" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>